<commit_message>
[FIXED] bugs, integrated codes
</commit_message>
<xml_diff>
--- a/Docu/calibration.xlsx
+++ b/Docu/calibration.xlsx
@@ -30,16 +30,16 @@
     <t>VB</t>
   </si>
   <si>
-    <t>VA-ADE</t>
+    <t>IA-RAW</t>
   </si>
   <si>
-    <t>VB-ADE</t>
+    <t>IB-RAW</t>
   </si>
   <si>
-    <t>IA-ADE</t>
+    <t>VA-RAW</t>
   </si>
   <si>
-    <t>IB-ADE</t>
+    <t>VB-RAW</t>
   </si>
 </sst>
 </file>
@@ -120,7 +120,7 @@
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="#,##0.000000" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -193,11 +193,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="98499904"/>
-        <c:axId val="98497600"/>
+        <c:axId val="86544896"/>
+        <c:axId val="86545472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98499904"/>
+        <c:axId val="86544896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -207,12 +207,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98497600"/>
+        <c:crossAx val="86545472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98497600"/>
+        <c:axId val="86545472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -223,7 +223,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98499904"/>
+        <c:crossAx val="86544896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -274,7 +274,7 @@
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.000000" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -347,11 +347,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124854272"/>
-        <c:axId val="98498752"/>
+        <c:axId val="86547200"/>
+        <c:axId val="86547776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124854272"/>
+        <c:axId val="86547200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -361,12 +361,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98498752"/>
+        <c:crossAx val="86547776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98498752"/>
+        <c:axId val="86547776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -377,7 +377,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124854272"/>
+        <c:crossAx val="86547200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -428,7 +428,7 @@
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="#,##0.0000000000" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -555,11 +555,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="151003136"/>
-        <c:axId val="124861760"/>
+        <c:axId val="44237952"/>
+        <c:axId val="44238528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="151003136"/>
+        <c:axId val="44237952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -569,12 +569,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124861760"/>
+        <c:crossAx val="44238528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124861760"/>
+        <c:axId val="44238528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -585,7 +585,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151003136"/>
+        <c:crossAx val="44237952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -636,7 +636,7 @@
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="#,##0.0000000000" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -763,11 +763,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="151008896"/>
-        <c:axId val="151008320"/>
+        <c:axId val="44240256"/>
+        <c:axId val="44240832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="151008896"/>
+        <c:axId val="44240256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -777,12 +777,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151008320"/>
+        <c:crossAx val="44240832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="151008320"/>
+        <c:axId val="44240832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -793,7 +793,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151008896"/>
+        <c:crossAx val="44240256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1229,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,25 +1241,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>

</xml_diff>